<commit_message>
Working example of ADC FFT
</commit_message>
<xml_diff>
--- a/MicroArraysFreqPhase/PIC_Calculations.xlsx
+++ b/MicroArraysFreqPhase/PIC_Calculations.xlsx
@@ -1,35 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Microchip\MicrophoneArray\microarrays\MicroArraysFreqPhase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{202F7752-CBBD-4CD2-A3FD-406FA662AF33}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD180E81-2827-4312-AA18-6DD6922FE2D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{B25A3D26-35BC-4A30-BE1F-6FDEA3B8CAC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{B25A3D26-35BC-4A30-BE1F-6FDEA3B8CAC4}"/>
   </bookViews>
   <sheets>
     <sheet name="CPU Clocking System" sheetId="2" r:id="rId1"/>
-    <sheet name="ADC" sheetId="1" r:id="rId2"/>
-    <sheet name="Time Analysis" sheetId="3" r:id="rId3"/>
-    <sheet name="Signal simulation" sheetId="4" r:id="rId4"/>
-    <sheet name="InputSignalSim" sheetId="5" r:id="rId5"/>
+    <sheet name="Timer" sheetId="6" r:id="rId2"/>
+    <sheet name="ADC" sheetId="1" r:id="rId3"/>
+    <sheet name="Time Analysis" sheetId="3" r:id="rId4"/>
+    <sheet name="Signal simulation" sheetId="4" r:id="rId5"/>
+    <sheet name="InputSignalSim" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>TCY</t>
   </si>
@@ -159,6 +165,9 @@
   <si>
     <t>fbin</t>
   </si>
+  <si>
+    <t>Interrupt Overhead</t>
+  </si>
 </sst>
 </file>
 
@@ -181,7 +190,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -189,13 +198,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -299,385 +337,385 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.2545454545454544E-5</c:v>
+                  <c:v>4.4155844155844159E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2509090909090909E-4</c:v>
+                  <c:v>8.8311688311688318E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8763636363636362E-4</c:v>
+                  <c:v>1.3246753246753249E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5018181818181818E-4</c:v>
+                  <c:v>1.7662337662337664E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.1272727272727273E-4</c:v>
+                  <c:v>2.2077922077922079E-5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.7527272727272724E-4</c:v>
+                  <c:v>2.6493506493506497E-5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.378181818181818E-4</c:v>
+                  <c:v>3.0909090909090909E-5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.0036363636363635E-4</c:v>
+                  <c:v>3.5324675324675327E-5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.6290909090909091E-4</c:v>
+                  <c:v>3.9740259740259746E-5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.2545454545454547E-4</c:v>
+                  <c:v>4.4155844155844157E-5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.8800000000000003E-4</c:v>
+                  <c:v>4.8571428571428576E-5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.5054545454545448E-4</c:v>
+                  <c:v>5.2987012987012994E-5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.1309090909090903E-4</c:v>
+                  <c:v>5.7402597402597406E-5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.7563636363636359E-4</c:v>
+                  <c:v>6.1818181818181818E-5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.3818181818181815E-4</c:v>
+                  <c:v>6.6233766233766243E-5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0007272727272727E-3</c:v>
+                  <c:v>7.0649350649350655E-5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0632727272727272E-3</c:v>
+                  <c:v>7.5064935064935066E-5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.1258181818181818E-3</c:v>
+                  <c:v>7.9480519480519492E-5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.1883636363636363E-3</c:v>
+                  <c:v>8.3896103896103903E-5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2509090909090909E-3</c:v>
+                  <c:v>8.8311688311688315E-5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.3134545454545454E-3</c:v>
+                  <c:v>9.272727272727274E-5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.3760000000000001E-3</c:v>
+                  <c:v>9.7142857142857152E-5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.4385454545454545E-3</c:v>
+                  <c:v>1.0155844155844156E-4</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.501090909090909E-3</c:v>
+                  <c:v>1.0597402597402599E-4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.5636363636363636E-3</c:v>
+                  <c:v>1.103896103896104E-4</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.6261818181818181E-3</c:v>
+                  <c:v>1.1480519480519481E-4</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.6887272727272727E-3</c:v>
+                  <c:v>1.1922077922077922E-4</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.7512727272727272E-3</c:v>
+                  <c:v>1.2363636363636364E-4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.8138181818181818E-3</c:v>
+                  <c:v>1.2805194805194807E-4</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.8763636363636363E-3</c:v>
+                  <c:v>1.3246753246753249E-4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.938909090909091E-3</c:v>
+                  <c:v>1.368831168831169E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.0014545454545454E-3</c:v>
+                  <c:v>1.4129870129870131E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.0639999999999999E-3</c:v>
+                  <c:v>1.4571428571428572E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.1265454545454543E-3</c:v>
+                  <c:v>1.5012987012987013E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.1890909090909092E-3</c:v>
+                  <c:v>1.5454545454545454E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.2516363636363636E-3</c:v>
+                  <c:v>1.5896103896103898E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.3141818181818181E-3</c:v>
+                  <c:v>1.6337662337662339E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.3767272727272725E-3</c:v>
+                  <c:v>1.6779220779220781E-4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.4392727272727274E-3</c:v>
+                  <c:v>1.7220779220779222E-4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.5018181818181819E-3</c:v>
+                  <c:v>1.7662337662337663E-4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.5643636363636363E-3</c:v>
+                  <c:v>1.8103896103896104E-4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.6269090909090908E-3</c:v>
+                  <c:v>1.8545454545454548E-4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.6894545454545452E-3</c:v>
+                  <c:v>1.8987012987012989E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.7520000000000001E-3</c:v>
+                  <c:v>1.942857142857143E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.8145454545454546E-3</c:v>
+                  <c:v>1.9870129870129872E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.877090909090909E-3</c:v>
+                  <c:v>2.0311688311688313E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.9396363636363635E-3</c:v>
+                  <c:v>2.0753246753246754E-4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.0021818181818179E-3</c:v>
+                  <c:v>2.1194805194805198E-4</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.0647272727272728E-3</c:v>
+                  <c:v>2.1636363636363639E-4</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.1272727272727272E-3</c:v>
+                  <c:v>2.207792207792208E-4</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.1898181818181817E-3</c:v>
+                  <c:v>2.2519480519480521E-4</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.2523636363636361E-3</c:v>
+                  <c:v>2.2961038961038962E-4</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>3.314909090909091E-3</c:v>
+                  <c:v>2.3402597402597404E-4</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>3.3774545454545455E-3</c:v>
+                  <c:v>2.3844155844155845E-4</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.4399999999999999E-3</c:v>
+                  <c:v>2.4285714285714289E-4</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3.5025454545454544E-3</c:v>
+                  <c:v>2.4727272727272727E-4</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3.5650909090909088E-3</c:v>
+                  <c:v>2.5168831168831168E-4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3.6276363636363637E-3</c:v>
+                  <c:v>2.5610389610389615E-4</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3.6901818181818181E-3</c:v>
+                  <c:v>2.6051948051948056E-4</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3.7527272727272726E-3</c:v>
+                  <c:v>2.6493506493506497E-4</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3.815272727272727E-3</c:v>
+                  <c:v>2.6935064935064938E-4</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3.8778181818181819E-3</c:v>
+                  <c:v>2.737662337662338E-4</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3.9403636363636359E-3</c:v>
+                  <c:v>2.7818181818181821E-4</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4.0029090909090908E-3</c:v>
+                  <c:v>2.8259740259740262E-4</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.0654545454545457E-3</c:v>
+                  <c:v>2.8701298701298703E-4</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.1279999999999997E-3</c:v>
+                  <c:v>2.9142857142857144E-4</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4.1905454545454546E-3</c:v>
+                  <c:v>2.9584415584415585E-4</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.2530909090909086E-3</c:v>
+                  <c:v>3.0025974025974027E-4</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4.3156363636363635E-3</c:v>
+                  <c:v>3.0467532467532468E-4</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>4.3781818181818184E-3</c:v>
+                  <c:v>3.0909090909090909E-4</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>4.4407272727272724E-3</c:v>
+                  <c:v>3.1350649350649355E-4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4.5032727272727273E-3</c:v>
+                  <c:v>3.1792207792207797E-4</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4.5658181818181813E-3</c:v>
+                  <c:v>3.2233766233766238E-4</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>4.6283636363636362E-3</c:v>
+                  <c:v>3.2675324675324679E-4</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>4.6909090909090911E-3</c:v>
+                  <c:v>3.311688311688312E-4</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4.7534545454545451E-3</c:v>
+                  <c:v>3.3558441558441561E-4</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4.816E-3</c:v>
+                  <c:v>3.4000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4.8785454545454549E-3</c:v>
+                  <c:v>3.4441558441558444E-4</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>4.9410909090909089E-3</c:v>
+                  <c:v>3.4883116883116885E-4</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>5.0036363636363637E-3</c:v>
+                  <c:v>3.5324675324675326E-4</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>5.0661818181818178E-3</c:v>
+                  <c:v>3.5766233766233767E-4</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>5.1287272727272726E-3</c:v>
+                  <c:v>3.6207792207792208E-4</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>5.1912727272727275E-3</c:v>
+                  <c:v>3.6649350649350649E-4</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>5.2538181818181815E-3</c:v>
+                  <c:v>3.7090909090909096E-4</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>5.3163636363636364E-3</c:v>
+                  <c:v>3.7532467532467537E-4</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>5.3789090909090904E-3</c:v>
+                  <c:v>3.7974025974025978E-4</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>5.4414545454545453E-3</c:v>
+                  <c:v>3.841558441558442E-4</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>5.5040000000000002E-3</c:v>
+                  <c:v>3.8857142857142861E-4</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>5.5665454545454542E-3</c:v>
+                  <c:v>3.9298701298701302E-4</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>5.6290909090909091E-3</c:v>
+                  <c:v>3.9740259740259743E-4</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>5.6916363636363631E-3</c:v>
+                  <c:v>4.0181818181818184E-4</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>5.754181818181818E-3</c:v>
+                  <c:v>4.0623376623376625E-4</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>5.8167272727272729E-3</c:v>
+                  <c:v>4.1064935064935067E-4</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>5.8792727272727269E-3</c:v>
+                  <c:v>4.1506493506493508E-4</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>5.9418181818181818E-3</c:v>
+                  <c:v>4.1948051948051949E-4</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>6.0043636363636358E-3</c:v>
+                  <c:v>4.2389610389610395E-4</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>6.0669090909090907E-3</c:v>
+                  <c:v>4.2831168831168837E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>6.1294545454545456E-3</c:v>
+                  <c:v>4.3272727272727278E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>6.1919999999999996E-3</c:v>
+                  <c:v>4.3714285714285719E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>6.2545454545454545E-3</c:v>
+                  <c:v>4.415584415584416E-4</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>6.3170909090909094E-3</c:v>
+                  <c:v>4.4597402597402601E-4</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>6.3796363636363634E-3</c:v>
+                  <c:v>4.5038961038961042E-4</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>6.4421818181818183E-3</c:v>
+                  <c:v>4.5480519480519484E-4</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>6.5047272727272723E-3</c:v>
+                  <c:v>4.5922077922077925E-4</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>6.5672727272727272E-3</c:v>
+                  <c:v>4.6363636363636366E-4</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>6.629818181818182E-3</c:v>
+                  <c:v>4.6805194805194807E-4</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>6.692363636363636E-3</c:v>
+                  <c:v>4.7246753246753248E-4</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>6.7549090909090909E-3</c:v>
+                  <c:v>4.7688311688311689E-4</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>6.8174545454545449E-3</c:v>
+                  <c:v>4.8129870129870136E-4</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>6.8799999999999998E-3</c:v>
+                  <c:v>4.8571428571428577E-4</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>6.9425454545454547E-3</c:v>
+                  <c:v>4.9012987012987013E-4</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>7.0050909090909087E-3</c:v>
+                  <c:v>4.9454545454545454E-4</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>7.0676363636363636E-3</c:v>
+                  <c:v>4.9896103896103895E-4</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>7.1301818181818176E-3</c:v>
+                  <c:v>5.0337662337662336E-4</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>7.1927272727272725E-3</c:v>
+                  <c:v>5.0779220779220778E-4</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>7.2552727272727274E-3</c:v>
+                  <c:v>5.122077922077923E-4</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>7.3178181818181814E-3</c:v>
+                  <c:v>5.1662337662337671E-4</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>7.3803636363636363E-3</c:v>
+                  <c:v>5.2103896103896112E-4</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>7.4429090909090912E-3</c:v>
+                  <c:v>5.2545454545454553E-4</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>7.5054545454545452E-3</c:v>
+                  <c:v>5.2987012987012994E-4</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>7.5680000000000001E-3</c:v>
+                  <c:v>5.3428571428571436E-4</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>7.6305454545454541E-3</c:v>
+                  <c:v>5.3870129870129877E-4</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>7.693090909090909E-3</c:v>
+                  <c:v>5.4311688311688318E-4</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>7.7556363636363639E-3</c:v>
+                  <c:v>5.4753246753246759E-4</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>7.8181818181818179E-3</c:v>
+                  <c:v>5.51948051948052E-4</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>7.8807272727272719E-3</c:v>
+                  <c:v>5.5636363636363641E-4</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>7.9432727272727276E-3</c:v>
+                  <c:v>5.6077922077922083E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -692,385 +730,385 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70751056426038361</c:v>
+                  <c:v>5.5459400993036104E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99999934746424279</c:v>
+                  <c:v>0.1107480916355004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70589404825489199</c:v>
+                  <c:v>0.16569588704271634</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-2.2847926692759288E-3</c:v>
+                  <c:v>0.22013365164435394</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.70912338685954623</c:v>
+                  <c:v>0.27389381980297228</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-0.99999412718329483</c:v>
+                  <c:v>0.32681091160012976</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.70427384728174414</c:v>
+                  <c:v>0.37872204220241307</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5695734112844331E-3</c:v>
+                  <c:v>0.42946742323950088</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.71073250763298745</c:v>
+                  <c:v>0.47889085465095904</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99998368664865012</c:v>
+                  <c:v>0.52684020548781152</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.70264996979884908</c:v>
+                  <c:v>0.57316788218892223</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-6.8543302988190195E-3</c:v>
+                  <c:v>0.61773128289077983</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.7123379181806383</c:v>
+                  <c:v>0.66039323637226965</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-0.99996802591481149</c:v>
+                  <c:v>0.70102242428331085</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-0.70102242428331263</c:v>
+                  <c:v>0.73949378535768784</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.1390514048030509E-3</c:v>
+                  <c:v>0.77568890036586691</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.71393961012179863</c:v>
+                  <c:v>0.80949635662286801</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.99994714506353211</c:v>
+                  <c:v>0.84081209092919318</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.69939121923138137</c:v>
+                  <c:v>0.86953970988920293</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1.1423724802338244E-2</c:v>
+                  <c:v>0.89559078662096292</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.7155375750951859</c:v>
+                  <c:v>0.91888513294425489</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-0.99992104420381611</c:v>
+                  <c:v>0.93935104620892351</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-0.69775636315840939</c:v>
+                  <c:v>0.95692553000379954</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.3708338564779807E-2</c:v>
+                  <c:v>0.9715544880668241</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.7171318047589611</c:v>
+                  <c:v>0.98319289079950301</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.99988972347191751</c:v>
+                  <c:v>0.99180491387313785</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.69611786459881164</c:v>
+                  <c:v>0.99736404850018856</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-1.5992880765799588E-2</c:v>
+                  <c:v>0.99985318303133919</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.71872229079079852</c:v>
+                  <c:v>0.99926465562710309</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.9998531830313393</c:v>
+                  <c:v>0.99560027784183713</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-0.69447573210601643</c:v>
+                  <c:v>0.98887132904757125</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.8277339479434121E-2</c:v>
+                  <c:v>0.97909852171481659</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.72030902488790349</c:v>
+                  <c:v>0.96631193765722401</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.99981142307283299</c:v>
+                  <c:v>0.95055093543633584</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.6928299742524251</c:v>
+                  <c:v>0.93186402921145239</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-2.0561702780159334E-2</c:v>
+                  <c:v>0.91030873940752666</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.7218919987670781</c:v>
+                  <c:v>0.8859514156607472</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.99976444381439733</c:v>
+                  <c:v>0.85886703258680275</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.69118059962935618</c:v>
+                  <c:v>0.82913895900048029</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.284595874294567E-2</c:v>
+                  <c:v>0.79685870129696068</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.72347120416474342</c:v>
+                  <c:v>0.76212562178471477</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.99971224550127757</c:v>
+                  <c:v>0.72504663283700677</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.68952761684701958</c:v>
+                  <c:v>0.68573586780343687</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-2.5130095443338118E-2</c:v>
+                  <c:v>0.64431432969449431</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-0.72504663283700577</c:v>
+                  <c:v>0.60090951872051668</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-0.99965482840596376</c:v>
+                  <c:v>0.55565503983152542</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-0.68787103453445286</c:v>
+                  <c:v>0.50869019146597683</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.7414100957472296E-2</c:v>
+                  <c:v>0.46015953677430993</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.72661827655966948</c:v>
+                  <c:v>0.41021245863711181</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.99959219282818945</c:v>
+                  <c:v>0.35900269984759869</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.68621086133948661</c:v>
+                  <c:v>0.30668788987379852</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-2.969796336221836E-2</c:v>
+                  <c:v>0.25342905965709966</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-0.72818612712831732</c:v>
+                  <c:v>0.19939014594067811</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-0.99952433909492988</c:v>
+                  <c:v>0.14473748665353955</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-0.68454710592869195</c:v>
+                  <c:v>8.963930890343362E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>3.1981670735143825E-2</c:v>
+                  <c:v>3.4265211154663869E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.72975017635830897</c:v>
+                  <c:v>-2.1214358815296808E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.99945126756040126</c:v>
+                  <c:v>-7.6628628573469304E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.68287977698735558</c:v>
+                  <c:v>-0.13180702668836025</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-3.4265211154653925E-2</c:v>
+                  <c:v>-0.18657970776825072</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-0.73131041608488201</c:v>
+                  <c:v>-0.24077807526464745</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-0.99937297860605745</c:v>
+                  <c:v>-0.2942353004316568</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-0.68120888321940343</c:v>
+                  <c:v>-0.34678683584385617</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3.6548572700025428E-2</c:v>
+                  <c:v>-0.39827092189200591</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.7328668381631317</c:v>
+                  <c:v>-0.44852908469754255</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.99928947264058965</c:v>
+                  <c:v>-0.49740662391322182</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.67953443334737085</c:v>
+                  <c:v>-0.54475308890839824</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-3.8831743451440491E-2</c:v>
+                  <c:v>-0.59042274187319743</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-0.73441943446808267</c:v>
+                  <c:v>-0.63427500641608803</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-0.99920075009992171</c:v>
+                  <c:v>-0.67617490027401916</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-0.67785643611237278</c:v>
+                  <c:v>-0.71599345080319499</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4.1114711490134064E-2</c:v>
+                  <c:v>-0.75360809197155576</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.73596819689475501</c:v>
+                  <c:v>-0.78890304163098079</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.99910681144721147</c:v>
+                  <c:v>-0.82176965790792089</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.67617490027402161</c:v>
+                  <c:v>-0.85210677361545673</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-4.3397464898321206E-2</c:v>
+                  <c:v>-0.87982100765741533</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-0.73751311735816871</c:v>
+                  <c:v>-0.90482705246601935</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-0.99900765717284468</c:v>
+                  <c:v>-0.92704793658829177</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-0.67448983461042811</c:v>
+                  <c:v>-0.94641526161295064</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>4.5679991759415513E-2</c:v>
+                  <c:v>-0.9628694127085089</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.73905418779338972</c:v>
+                  <c:v>-0.9763597421245116</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.99890328779443582</c:v>
+                  <c:v>-0.98684472509107801</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.67280124791808804</c:v>
+                  <c:v>-0.99429208763687249</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>-4.7962280157963534E-2</c:v>
+                  <c:v>-0.99867890593206143</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>-0.74059140015560199</c:v>
+                  <c:v>-0.99999167685047219</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>-0.99879370385682154</c:v>
+                  <c:v>-0.99822635953375283</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>-0.67110914901193552</c:v>
+                  <c:v>-0.99338838782959382</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>5.024431817977084E-2</c:v>
+                  <c:v>-0.98549265356572668</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.74212474642010551</c:v>
+                  <c:v>-0.97456346071118227</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.99867890593206166</c:v>
+                  <c:v>-0.96063445056590702</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.66941354672519249</c:v>
+                  <c:v>-0.94374849820901208</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>-5.2526093911935856E-2</c:v>
+                  <c:v>-0.92395758052439747</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>-0.74365421858241576</c:v>
+                  <c:v>-0.90132261620998577</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>-0.9985588946194347</c:v>
+                  <c:v>-0.875913278263035</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>-0.66771444990936357</c:v>
+                  <c:v>-0.84780777951871922</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>5.4807595442954632E-2</c:v>
+                  <c:v>-0.81709263190211612</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.74517980865824363</c:v>
+                  <c:v>-0.7838623801346567</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.99843367054543253</c:v>
+                  <c:v>-0.7482193107147016</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.66601186743425977</c:v>
+                  <c:v>-0.71027313706805684</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>-5.7088810862754608E-2</c:v>
+                  <c:v>-0.6701406618375596</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>-0.7467015086835751</c:v>
+                  <c:v>-0.62794541735124088</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>-0.99830323436376189</c:v>
+                  <c:v>-0.58381728537575706</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>-0.66430580818781404</c:v>
+                  <c:v>-0.53789209732552679</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>5.9369728262728419E-2</c:v>
+                  <c:v>-0.49031121615816797</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>0.74821931071469394</c:v>
+                  <c:v>-0.44122110124322145</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>0.99816758675533435</c:v>
+                  <c:v>-0.39077285754353874</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>0.66259628107616175</c:v>
+                  <c:v>-0.33912177049699727</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>-6.1650335735838648E-2</c:v>
+                  <c:v>-0.2864268280302486</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>-0.7497332068282514</c:v>
+                  <c:v>-0.23285023117577217</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>-0.99802672842827211</c:v>
+                  <c:v>-0.17855689479863687</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>-0.66088329502349952</c:v>
+                  <c:v>-0.123713939969764</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>6.393062137665162E-2</c:v>
+                  <c:v>-6.849017954824671E-2</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>0.75124318912128873</c:v>
+                  <c:v>-1.3055598556147987E-2</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>0.99788066011789434</c:v>
+                  <c:v>4.2419169054747352E-2</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>0.65916685897211214</c:v>
+                  <c:v>9.7763365633669053E-2</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>-6.6210573281456214E-2</c:v>
+                  <c:v>0.15280663544235026</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>-0.75274924971125945</c:v>
+                  <c:v>0.20737954902938052</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>-0.99772938258671795</c:v>
+                  <c:v>0.26131412475335447</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>-0.65744698188228401</c:v>
+                  <c:v>0.31444434584948794</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>6.8490179548226851E-2</c:v>
+                  <c:v>0.36660667144812081</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>0.7542513807360991</c:v>
+                  <c:v>0.41764053997213119</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>0.99757289662445581</c:v>
+                  <c:v>0.46738886336375562</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>0.65572367273227306</c:v>
+                  <c:v>0.51569851061951333</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>-7.0769428276813109E-2</c:v>
+                  <c:v>0.56242077914486777</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>-0.75574957435424728</c:v>
+                  <c:v>0.60741185247774776</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>-0.9974112030480099</c:v>
+                  <c:v>0.650533242971987</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>-0.65399694051822188</c:v>
+                  <c:v>0.69165221807807031</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6597,10 +6635,10 @@
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>14737</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>714031</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>129571</xdr:rowOff>
+      <xdr:rowOff>126396</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6642,7 +6680,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>101500</xdr:colOff>
+      <xdr:colOff>45144</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>132869</xdr:rowOff>
     </xdr:to>
@@ -6686,14 +6724,63 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>646190</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>56148</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A939A221-D568-45F0-A341-4666DFB1712F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1085850"/>
+          <a:ext cx="12076190" cy="8019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>319512</xdr:colOff>
+      <xdr:colOff>316337</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>173728</xdr:rowOff>
+      <xdr:rowOff>154678</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6729,7 +6816,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6772,20 +6859,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>536575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>536575</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6812,16 +6899,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>536575</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>625475</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>536575</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>625475</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7148,13 +7235,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D670349-287E-4B94-99F6-4B80420353F2}">
   <dimension ref="A58:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -7183,7 +7270,7 @@
       </c>
       <c r="G59">
         <f>B59/B64</f>
-        <v>2750000</v>
+        <v>5500000</v>
       </c>
       <c r="H59" t="b">
         <f>AND(G59&gt;D59,G59&lt;E59)</f>
@@ -7195,7 +7282,7 @@
         <v>15</v>
       </c>
       <c r="B60">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D60" s="1">
         <v>120000000</v>
@@ -7208,7 +7295,7 @@
       </c>
       <c r="G60">
         <f>B59*(B66/B64)</f>
-        <v>159500000</v>
+        <v>231000000</v>
       </c>
       <c r="H60" t="b">
         <f>AND(G60&gt;D60,G60&lt;E60)</f>
@@ -7220,7 +7307,7 @@
         <v>16</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -7233,7 +7320,7 @@
       </c>
       <c r="G61">
         <f>B68</f>
-        <v>79750000</v>
+        <v>115500000</v>
       </c>
       <c r="H61" t="b">
         <f>G61&lt;E61</f>
@@ -7254,7 +7341,7 @@
       </c>
       <c r="B64">
         <f>B61+2</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -7272,7 +7359,7 @@
       </c>
       <c r="B66">
         <f>B60+2</f>
-        <v>58</v>
+        <v>42</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
@@ -7281,7 +7368,7 @@
       </c>
       <c r="B68">
         <f>B59*(B66/(B64*B65))</f>
-        <v>79750000</v>
+        <v>115500000</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
@@ -7290,7 +7377,7 @@
       </c>
       <c r="B70">
         <f>B68/2</f>
-        <v>39875000</v>
+        <v>57750000</v>
       </c>
     </row>
   </sheetData>
@@ -7301,11 +7388,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91A7E69-E977-44DF-AABD-3B9102489A54}">
-  <dimension ref="A2:J15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444216E4-BC63-4907-9153-1989B7CA357E}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91A7E69-E977-44DF-AABD-3B9102489A54}">
+  <dimension ref="A2:Q31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7314,46 +7416,67 @@
     <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.453125" customWidth="1"/>
     <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
         <f>'CPU Clocking System'!B70</f>
-        <v>39875000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>57750000</v>
+      </c>
+      <c r="C2">
+        <v>57750000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
         <f>1/B2</f>
-        <v>2.5078369905956112E-8</v>
+        <v>1.7316017316017315E-8</v>
       </c>
       <c r="E3">
         <v>370</v>
       </c>
       <c r="F3">
         <f>E3*B3</f>
-        <v>9.2789968652037618E-6</v>
+        <v>6.4069264069264066E-6</v>
       </c>
       <c r="G3">
         <f>1/F3</f>
-        <v>107770.27027027027</v>
+        <v>156081.08108108109</v>
       </c>
       <c r="I3">
         <v>18985404</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="M3">
+        <f>1/(44100)</f>
+        <v>2.2675736961451248E-5</v>
+      </c>
+      <c r="N3">
+        <f>M3/B3</f>
+        <v>1309.5238095238096</v>
+      </c>
+      <c r="P3">
+        <f>M3*128</f>
+        <v>2.9024943310657597E-3</v>
+      </c>
+      <c r="Q3">
+        <f>P3*2</f>
+        <v>5.8049886621315194E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D4" t="b">
         <f>B4&lt;=31</f>
@@ -7367,12 +7490,12 @@
         <v>3520149</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="I5">
         <v>24265390</v>
@@ -7382,13 +7505,13 @@
         <v>1759837</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <f>B3*(B5+1)</f>
-        <v>1.0783699059561129E-6</v>
+        <v>8.6580086580086576E-8</v>
       </c>
       <c r="C6" s="1">
         <v>7.6000000000000006E-8</v>
@@ -7404,26 +7527,33 @@
         <f>I6-I5</f>
         <v>1759773</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="O6" s="1">
+        <v>1.9029999999999999E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <f>12*B6</f>
-        <v>1.2940438871473354E-5</v>
+        <v>1.038961038961039E-6</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="O7">
+        <f>B7*3</f>
+        <v>3.1168831168831169E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
         <f>B4*B6</f>
-        <v>1.078369905956113E-5</v>
+        <v>2.5974025974025974E-7</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -7432,8 +7562,16 @@
         <f>B8&gt;(2*B6)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="O8" s="1">
+        <f>O7+O6</f>
+        <v>2.2146883116883116E-5</v>
+      </c>
+      <c r="P8" s="2">
+        <f>1/O8</f>
+        <v>45153.080671549455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -7443,75 +7581,131 @@
       <c r="C9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="M9">
+        <f>M3/B10</f>
+        <v>5.1353874883286643</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
         <f>B8+(B9*B7)</f>
-        <v>6.2545454545454544E-5</v>
+        <v>4.4155844155844159E-6</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
         <f>1/B10</f>
-        <v>15988.372093023256</v>
+        <v>226470.5882352941</v>
       </c>
       <c r="C12">
         <f>B12/1000</f>
-        <v>15.988372093023255</v>
+        <v>226.47058823529409</v>
       </c>
       <c r="F12">
         <f>B10*128</f>
-        <v>8.0058181818181817E-3</v>
+        <v>5.6519480519480524E-4</v>
       </c>
       <c r="J12">
         <f>J6/1000000000</f>
         <v>1.7597730000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B13">
         <f>1/B7</f>
-        <v>77277.13178294574</v>
+        <v>962500</v>
       </c>
       <c r="C13">
         <f>B13/1000</f>
-        <v>77.277131782945744</v>
+        <v>962.5</v>
       </c>
       <c r="F13">
         <f>1/B13</f>
-        <v>1.2940438871473354E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1.038961038961039E-6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="M14">
+        <f>M3*128</f>
+        <v>2.9024943310657597E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="E15" t="s">
         <v>25</v>
       </c>
       <c r="F15">
         <f>B10*128</f>
-        <v>8.0058181818181817E-3</v>
+        <v>5.6519480519480524E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="13:16" x14ac:dyDescent="0.35">
+      <c r="M20">
+        <f>B3*13</f>
+        <v>2.2510822510822508E-7</v>
+      </c>
+      <c r="N20">
+        <f>M20*128</f>
+        <v>2.8813852813852811E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="13:16" x14ac:dyDescent="0.35">
+      <c r="N21">
+        <f>M20*128</f>
+        <v>2.8813852813852811E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="13:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N22">
+        <f>M20</f>
+        <v>2.2510822510822508E-7</v>
+      </c>
+    </row>
+    <row r="23" spans="13:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="M23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N23" s="4">
+        <f>SUM(N20:N22)</f>
+        <v>5.7852813852813844E-5</v>
+      </c>
+      <c r="P23">
+        <f>M14-N23</f>
+        <v>2.8446415172129458E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="13:16" x14ac:dyDescent="0.35">
+      <c r="M30">
+        <v>26.548462000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="13:16" x14ac:dyDescent="0.35">
+      <c r="M31">
+        <v>26.372679999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0871B62A-0198-4755-A09B-E37BC7CBD8D4}">
   <dimension ref="A2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7585,7 +7779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A938EB4D-6CD0-4E89-9C8C-754601A337CD}">
   <dimension ref="A1:M131"/>
   <sheetViews>
@@ -7604,14 +7798,14 @@
       </c>
       <c r="B1">
         <f>1/ADC!B12</f>
-        <v>6.2545454545454544E-5</v>
+        <v>4.4155844155844159E-6</v>
       </c>
       <c r="L1" t="s">
         <v>40</v>
       </c>
       <c r="M1">
         <f>1/B1</f>
-        <v>15988.372093023256</v>
+        <v>226470.5882352941</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -7657,7 +7851,7 @@
       </c>
       <c r="M4">
         <f>M1/(M2/2)</f>
-        <v>249.81831395348837</v>
+        <v>3538.6029411764703</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
@@ -7666,11 +7860,11 @@
       </c>
       <c r="B5">
         <f t="shared" ref="B5:B68" si="0">A5*$B$1</f>
-        <v>6.2545454545454544E-5</v>
+        <v>4.4155844155844159E-6</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C68" si="1">SIN(2*PI()*$B$2*B5)</f>
-        <v>0.70751056426038361</v>
+        <v>5.5459400993036104E-2</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -7682,11 +7876,11 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>1.2509090909090909E-4</v>
+        <v>8.8311688311688318E-6</v>
       </c>
       <c r="C6">
         <f t="shared" si="1"/>
-        <v>0.99999934746424279</v>
+        <v>0.1107480916355004</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -7698,11 +7892,11 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>1.8763636363636362E-4</v>
+        <v>1.3246753246753249E-5</v>
       </c>
       <c r="C7">
         <f t="shared" si="1"/>
-        <v>0.70589404825489199</v>
+        <v>0.16569588704271634</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -7721,11 +7915,11 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>2.5018181818181818E-4</v>
+        <v>1.7662337662337664E-5</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>-2.2847926692759288E-3</v>
+        <v>0.22013365164435394</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -7735,7 +7929,7 @@
       </c>
       <c r="M8">
         <f t="shared" ref="M8:M70" si="2">L8*$M$4</f>
-        <v>249.81831395348837</v>
+        <v>3538.6029411764703</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -7744,11 +7938,11 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>3.1272727272727273E-4</v>
+        <v>2.2077922077922079E-5</v>
       </c>
       <c r="C9">
         <f t="shared" si="1"/>
-        <v>-0.70912338685954623</v>
+        <v>0.27389381980297228</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -7758,7 +7952,7 @@
       </c>
       <c r="M9">
         <f t="shared" si="2"/>
-        <v>499.63662790697674</v>
+        <v>7077.2058823529405</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -7767,11 +7961,11 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>3.7527272727272724E-4</v>
+        <v>2.6493506493506497E-5</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>-0.99999412718329483</v>
+        <v>0.32681091160012976</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -7781,7 +7975,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>749.45494186046517</v>
+        <v>10615.808823529411</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -7790,11 +7984,11 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>4.378181818181818E-4</v>
+        <v>3.0909090909090909E-5</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>-0.70427384728174414</v>
+        <v>0.37872204220241307</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -7804,7 +7998,7 @@
       </c>
       <c r="M11">
         <f t="shared" si="2"/>
-        <v>999.27325581395348</v>
+        <v>14154.411764705881</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -7813,11 +8007,11 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>5.0036363636363635E-4</v>
+        <v>3.5324675324675327E-5</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>4.5695734112844331E-3</v>
+        <v>0.42946742323950088</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -7827,7 +8021,7 @@
       </c>
       <c r="M12">
         <f t="shared" si="2"/>
-        <v>1249.0915697674418</v>
+        <v>17693.01470588235</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -7836,11 +8030,11 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>5.6290909090909091E-4</v>
+        <v>3.9740259740259746E-5</v>
       </c>
       <c r="C13">
         <f t="shared" si="1"/>
-        <v>0.71073250763298745</v>
+        <v>0.47889085465095904</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -7850,7 +8044,7 @@
       </c>
       <c r="M13">
         <f t="shared" si="2"/>
-        <v>1498.9098837209303</v>
+        <v>21231.617647058822</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -7859,11 +8053,11 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>6.2545454545454547E-4</v>
+        <v>4.4155844155844157E-5</v>
       </c>
       <c r="C14">
         <f t="shared" si="1"/>
-        <v>0.99998368664865012</v>
+        <v>0.52684020548781152</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -7873,7 +8067,7 @@
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>1748.7281976744187</v>
+        <v>24770.220588235294</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -7882,11 +8076,11 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>6.8800000000000003E-4</v>
+        <v>4.8571428571428576E-5</v>
       </c>
       <c r="C15">
         <f t="shared" si="1"/>
-        <v>0.70264996979884908</v>
+        <v>0.57316788218892223</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -7896,7 +8090,7 @@
       </c>
       <c r="M15">
         <f t="shared" si="2"/>
-        <v>1998.546511627907</v>
+        <v>28308.823529411762</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -7905,11 +8099,11 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>7.5054545454545448E-4</v>
+        <v>5.2987012987012994E-5</v>
       </c>
       <c r="C16">
         <f t="shared" si="1"/>
-        <v>-6.8543302988190195E-3</v>
+        <v>0.61773128289077983</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -7919,7 +8113,7 @@
       </c>
       <c r="M16">
         <f t="shared" si="2"/>
-        <v>2248.3648255813955</v>
+        <v>31847.426470588231</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
@@ -7928,11 +8122,11 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>8.1309090909090903E-4</v>
+        <v>5.7402597402597406E-5</v>
       </c>
       <c r="C17">
         <f t="shared" si="1"/>
-        <v>-0.7123379181806383</v>
+        <v>0.66039323637226965</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -7942,7 +8136,7 @@
       </c>
       <c r="M17">
         <f t="shared" si="2"/>
-        <v>2498.1831395348836</v>
+        <v>35386.029411764699</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
@@ -7951,11 +8145,11 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>8.7563636363636359E-4</v>
+        <v>6.1818181818181818E-5</v>
       </c>
       <c r="C18">
         <f t="shared" si="1"/>
-        <v>-0.99996802591481149</v>
+        <v>0.70102242428331085</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -7965,7 +8159,7 @@
       </c>
       <c r="M18">
         <f t="shared" si="2"/>
-        <v>2748.0014534883721</v>
+        <v>38924.632352941175</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
@@ -7974,11 +8168,11 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>9.3818181818181815E-4</v>
+        <v>6.6233766233766243E-5</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>-0.70102242428331263</v>
+        <v>0.73949378535768784</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -7988,7 +8182,7 @@
       </c>
       <c r="M19">
         <f t="shared" si="2"/>
-        <v>2997.8197674418607</v>
+        <v>42463.235294117643</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
@@ -7997,11 +8191,11 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>1.0007272727272727E-3</v>
+        <v>7.0649350649350655E-5</v>
       </c>
       <c r="C20">
         <f t="shared" si="1"/>
-        <v>9.1390514048030509E-3</v>
+        <v>0.77568890036586691</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -8011,7 +8205,7 @@
       </c>
       <c r="M20">
         <f t="shared" si="2"/>
-        <v>3247.6380813953488</v>
+        <v>46001.838235294112</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
@@ -8020,11 +8214,11 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>1.0632727272727272E-3</v>
+        <v>7.5064935064935066E-5</v>
       </c>
       <c r="C21">
         <f t="shared" si="1"/>
-        <v>0.71393961012179863</v>
+        <v>0.80949635662286801</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -8034,7 +8228,7 @@
       </c>
       <c r="M21">
         <f t="shared" si="2"/>
-        <v>3497.4563953488373</v>
+        <v>49540.441176470587</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
@@ -8043,11 +8237,11 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>1.1258181818181818E-3</v>
+        <v>7.9480519480519492E-5</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
-        <v>0.99994714506353211</v>
+        <v>0.84081209092919318</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -8057,7 +8251,7 @@
       </c>
       <c r="M22">
         <f t="shared" si="2"/>
-        <v>3747.2747093023254</v>
+        <v>53079.044117647056</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
@@ -8066,11 +8260,11 @@
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>1.1883636363636363E-3</v>
+        <v>8.3896103896103903E-5</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>0.69939121923138137</v>
+        <v>0.86953970988920293</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -8080,7 +8274,7 @@
       </c>
       <c r="M23">
         <f t="shared" si="2"/>
-        <v>3997.0930232558139</v>
+        <v>56617.647058823524</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
@@ -8089,11 +8283,11 @@
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>1.2509090909090909E-3</v>
+        <v>8.8311688311688315E-5</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>-1.1423724802338244E-2</v>
+        <v>0.89559078662096292</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -8103,7 +8297,7 @@
       </c>
       <c r="M24">
         <f t="shared" si="2"/>
-        <v>4246.9113372093025</v>
+        <v>60156.249999999993</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
@@ -8112,11 +8306,11 @@
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>1.3134545454545454E-3</v>
+        <v>9.272727272727274E-5</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>-0.7155375750951859</v>
+        <v>0.91888513294425489</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -8126,7 +8320,7 @@
       </c>
       <c r="M25">
         <f t="shared" si="2"/>
-        <v>4496.729651162791</v>
+        <v>63694.852941176461</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
@@ -8135,11 +8329,11 @@
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>1.3760000000000001E-3</v>
+        <v>9.7142857142857152E-5</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>-0.99992104420381611</v>
+        <v>0.93935104620892351</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -8149,7 +8343,7 @@
       </c>
       <c r="M26">
         <f t="shared" si="2"/>
-        <v>4746.5479651162786</v>
+        <v>67233.455882352937</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
@@ -8158,11 +8352,11 @@
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>1.4385454545454545E-3</v>
+        <v>1.0155844155844156E-4</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>-0.69775636315840939</v>
+        <v>0.95692553000379954</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -8172,7 +8366,7 @@
       </c>
       <c r="M27">
         <f t="shared" si="2"/>
-        <v>4996.3662790697672</v>
+        <v>70772.058823529398</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
@@ -8181,11 +8375,11 @@
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>1.501090909090909E-3</v>
+        <v>1.0597402597402599E-4</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>1.3708338564779807E-2</v>
+        <v>0.9715544880668241</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -8195,7 +8389,7 @@
       </c>
       <c r="M28">
         <f t="shared" si="2"/>
-        <v>5246.1845930232557</v>
+        <v>74310.661764705874</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
@@ -8204,11 +8398,11 @@
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>1.5636363636363636E-3</v>
+        <v>1.103896103896104E-4</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>0.7171318047589611</v>
+        <v>0.98319289079950301</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -8218,7 +8412,7 @@
       </c>
       <c r="M29">
         <f t="shared" si="2"/>
-        <v>5496.0029069767443</v>
+        <v>77849.26470588235</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
@@ -8227,11 +8421,11 @@
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>1.6261818181818181E-3</v>
+        <v>1.1480519480519481E-4</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>0.99988972347191751</v>
+        <v>0.99180491387313785</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -8241,7 +8435,7 @@
       </c>
       <c r="M30">
         <f t="shared" si="2"/>
-        <v>5745.8212209302328</v>
+        <v>81387.867647058811</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
@@ -8250,11 +8444,11 @@
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>1.6887272727272727E-3</v>
+        <v>1.1922077922077922E-4</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>0.69611786459881164</v>
+        <v>0.99736404850018856</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -8264,7 +8458,7 @@
       </c>
       <c r="M31">
         <f t="shared" si="2"/>
-        <v>5995.6395348837214</v>
+        <v>84926.470588235286</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
@@ -8273,11 +8467,11 @@
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>1.7512727272727272E-3</v>
+        <v>1.2363636363636364E-4</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>-1.5992880765799588E-2</v>
+        <v>0.99985318303133919</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -8287,7 +8481,7 @@
       </c>
       <c r="M32">
         <f t="shared" si="2"/>
-        <v>6245.457848837209</v>
+        <v>88465.073529411762</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
@@ -8296,11 +8490,11 @@
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>1.8138181818181818E-3</v>
+        <v>1.2805194805194807E-4</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>-0.71872229079079852</v>
+        <v>0.99926465562710309</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -8310,7 +8504,7 @@
       </c>
       <c r="M33">
         <f t="shared" si="2"/>
-        <v>6495.2761627906975</v>
+        <v>92003.676470588223</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
@@ -8319,11 +8513,11 @@
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>1.8763636363636363E-3</v>
+        <v>1.3246753246753249E-4</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>-0.9998531830313393</v>
+        <v>0.99560027784183713</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -8333,7 +8527,7 @@
       </c>
       <c r="M34">
         <f t="shared" si="2"/>
-        <v>6745.0944767441861</v>
+        <v>95542.279411764699</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
@@ -8342,11 +8536,11 @@
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>1.938909090909091E-3</v>
+        <v>1.368831168831169E-4</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>-0.69447573210601643</v>
+        <v>0.98887132904757125</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -8356,7 +8550,7 @@
       </c>
       <c r="M35">
         <f t="shared" si="2"/>
-        <v>6994.9127906976746</v>
+        <v>99080.882352941175</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
@@ -8365,11 +8559,11 @@
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>2.0014545454545454E-3</v>
+        <v>1.4129870129870131E-4</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>1.8277339479434121E-2</v>
+        <v>0.97909852171481659</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -8379,7 +8573,7 @@
       </c>
       <c r="M36">
         <f t="shared" si="2"/>
-        <v>7244.7311046511632</v>
+        <v>102619.48529411764</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
@@ -8388,11 +8582,11 @@
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>2.0639999999999999E-3</v>
+        <v>1.4571428571428572E-4</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>0.72030902488790349</v>
+        <v>0.96631193765722401</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -8402,7 +8596,7 @@
       </c>
       <c r="M37">
         <f t="shared" si="2"/>
-        <v>7494.5494186046508</v>
+        <v>106158.08823529411</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
@@ -8411,11 +8605,11 @@
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>2.1265454545454543E-3</v>
+        <v>1.5012987012987013E-4</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>0.99981142307283299</v>
+        <v>0.95055093543633584</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -8425,7 +8619,7 @@
       </c>
       <c r="M38">
         <f t="shared" si="2"/>
-        <v>7744.3677325581393</v>
+        <v>109696.69117647057</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
@@ -8434,11 +8628,11 @@
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>2.1890909090909092E-3</v>
+        <v>1.5454545454545454E-4</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>0.6928299742524251</v>
+        <v>0.93186402921145239</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -8448,7 +8642,7 @@
       </c>
       <c r="M39">
         <f t="shared" si="2"/>
-        <v>7994.1860465116279</v>
+        <v>113235.29411764705</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
@@ -8457,11 +8651,11 @@
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>2.2516363636363636E-3</v>
+        <v>1.5896103896103898E-4</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>-2.0561702780159334E-2</v>
+        <v>0.91030873940752666</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -8471,7 +8665,7 @@
       </c>
       <c r="M40">
         <f t="shared" si="2"/>
-        <v>8244.0043604651164</v>
+        <v>116773.89705882352</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
@@ -8480,11 +8674,11 @@
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>2.3141818181818181E-3</v>
+        <v>1.6337662337662339E-4</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>-0.7218919987670781</v>
+        <v>0.8859514156607472</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -8494,7 +8688,7 @@
       </c>
       <c r="M41">
         <f t="shared" si="2"/>
-        <v>8493.8226744186049</v>
+        <v>120312.49999999999</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
@@ -8503,11 +8697,11 @@
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>2.3767272727272725E-3</v>
+        <v>1.6779220779220781E-4</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>-0.99976444381439733</v>
+        <v>0.85886703258680275</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -8517,7 +8711,7 @@
       </c>
       <c r="M42">
         <f t="shared" si="2"/>
-        <v>8743.6409883720935</v>
+        <v>123851.10294117646</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
@@ -8526,11 +8720,11 @@
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>2.4392727272727274E-3</v>
+        <v>1.7220779220779222E-4</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>-0.69118059962935618</v>
+        <v>0.82913895900048029</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -8540,7 +8734,7 @@
       </c>
       <c r="M43">
         <f t="shared" si="2"/>
-        <v>8993.459302325582</v>
+        <v>127389.70588235292</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
@@ -8549,11 +8743,11 @@
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>2.5018181818181819E-3</v>
+        <v>1.7662337662337663E-4</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>2.284595874294567E-2</v>
+        <v>0.79685870129696068</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -8563,7 +8757,7 @@
       </c>
       <c r="M44">
         <f t="shared" si="2"/>
-        <v>9243.2776162790706</v>
+        <v>130928.3088235294</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
@@ -8572,11 +8766,11 @@
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>2.5643636363636363E-3</v>
+        <v>1.8103896103896104E-4</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>0.72347120416474342</v>
+        <v>0.76212562178471477</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -8586,7 +8780,7 @@
       </c>
       <c r="M45">
         <f t="shared" si="2"/>
-        <v>9493.0959302325573</v>
+        <v>134466.91176470587</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
@@ -8595,11 +8789,11 @@
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>2.6269090909090908E-3</v>
+        <v>1.8545454545454548E-4</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>0.99971224550127757</v>
+        <v>0.72504663283700677</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -8609,7 +8803,7 @@
       </c>
       <c r="M46">
         <f t="shared" si="2"/>
-        <v>9742.9142441860458</v>
+        <v>138005.51470588235</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
@@ -8618,11 +8812,11 @@
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>2.6894545454545452E-3</v>
+        <v>1.8987012987012989E-4</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>0.68952761684701958</v>
+        <v>0.68573586780343687</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -8632,7 +8826,7 @@
       </c>
       <c r="M47">
         <f t="shared" si="2"/>
-        <v>9992.7325581395344</v>
+        <v>141544.1176470588</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
@@ -8641,11 +8835,11 @@
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>2.7520000000000001E-3</v>
+        <v>1.942857142857143E-4</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>-2.5130095443338118E-2</v>
+        <v>0.64431432969449431</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -8655,7 +8849,7 @@
       </c>
       <c r="M48">
         <f t="shared" si="2"/>
-        <v>10242.550872093023</v>
+        <v>145082.72058823527</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
@@ -8664,11 +8858,11 @@
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>2.8145454545454546E-3</v>
+        <v>1.9870129870129872E-4</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>-0.72504663283700577</v>
+        <v>0.60090951872051668</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -8678,7 +8872,7 @@
       </c>
       <c r="M49">
         <f t="shared" si="2"/>
-        <v>10492.369186046511</v>
+        <v>148621.32352941175</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
@@ -8687,11 +8881,11 @@
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>2.877090909090909E-3</v>
+        <v>2.0311688311688313E-4</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>-0.99965482840596376</v>
+        <v>0.55565503983152542</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -8701,7 +8895,7 @@
       </c>
       <c r="M50">
         <f t="shared" si="2"/>
-        <v>10742.1875</v>
+        <v>152159.92647058822</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
@@ -8710,11 +8904,11 @@
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>2.9396363636363635E-3</v>
+        <v>2.0753246753246754E-4</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>-0.68787103453445286</v>
+        <v>0.50869019146597683</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -8724,7 +8918,7 @@
       </c>
       <c r="M51">
         <f t="shared" si="2"/>
-        <v>10992.005813953489</v>
+        <v>155698.5294117647</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
@@ -8733,11 +8927,11 @@
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>3.0021818181818179E-3</v>
+        <v>2.1194805194805198E-4</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>2.7414100957472296E-2</v>
+        <v>0.46015953677430993</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -8747,7 +8941,7 @@
       </c>
       <c r="M52">
         <f t="shared" si="2"/>
-        <v>11241.824127906977</v>
+        <v>159237.13235294117</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
@@ -8756,11 +8950,11 @@
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>3.0647272727272728E-3</v>
+        <v>2.1636363636363639E-4</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>0.72661827655966948</v>
+        <v>0.41021245863711181</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -8770,7 +8964,7 @@
       </c>
       <c r="M53">
         <f t="shared" si="2"/>
-        <v>11491.642441860466</v>
+        <v>162775.73529411762</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
@@ -8779,11 +8973,11 @@
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>3.1272727272727272E-3</v>
+        <v>2.207792207792208E-4</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>0.99959219282818945</v>
+        <v>0.35900269984759869</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -8793,7 +8987,7 @@
       </c>
       <c r="M54">
         <f t="shared" si="2"/>
-        <v>11741.460755813954</v>
+        <v>166314.3382352941</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
@@ -8802,11 +8996,11 @@
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>3.1898181818181817E-3</v>
+        <v>2.2519480519480521E-4</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>0.68621086133948661</v>
+        <v>0.30668788987379852</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -8816,7 +9010,7 @@
       </c>
       <c r="M55">
         <f t="shared" si="2"/>
-        <v>11991.279069767443</v>
+        <v>169852.94117647057</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
@@ -8825,11 +9019,11 @@
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>3.2523636363636361E-3</v>
+        <v>2.2961038961038962E-4</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
-        <v>-2.969796336221836E-2</v>
+        <v>0.25342905965709966</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -8839,7 +9033,7 @@
       </c>
       <c r="M56">
         <f t="shared" si="2"/>
-        <v>12241.097383720929</v>
+        <v>173391.54411764705</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
@@ -8848,11 +9042,11 @@
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>3.314909090909091E-3</v>
+        <v>2.3402597402597404E-4</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
-        <v>-0.72818612712831732</v>
+        <v>0.19939014594067811</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -8862,7 +9056,7 @@
       </c>
       <c r="M57">
         <f t="shared" si="2"/>
-        <v>12490.915697674418</v>
+        <v>176930.14705882352</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
@@ -8871,11 +9065,11 @@
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>3.3774545454545455E-3</v>
+        <v>2.3844155844155845E-4</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
-        <v>-0.99952433909492988</v>
+        <v>0.14473748665353955</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -8885,7 +9079,7 @@
       </c>
       <c r="M58">
         <f t="shared" si="2"/>
-        <v>12740.734011627907</v>
+        <v>180468.74999999997</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
@@ -8894,11 +9088,11 @@
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>3.4399999999999999E-3</v>
+        <v>2.4285714285714289E-4</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
-        <v>-0.68454710592869195</v>
+        <v>8.963930890343362E-2</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -8908,7 +9102,7 @@
       </c>
       <c r="M59">
         <f t="shared" si="2"/>
-        <v>12990.552325581395</v>
+        <v>184007.35294117645</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
@@ -8917,11 +9111,11 @@
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>3.5025454545454544E-3</v>
+        <v>2.4727272727272727E-4</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
-        <v>3.1981670735143825E-2</v>
+        <v>3.4265211154663869E-2</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -8931,7 +9125,7 @@
       </c>
       <c r="M60">
         <f t="shared" si="2"/>
-        <v>13240.370639534884</v>
+        <v>187545.95588235292</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
@@ -8940,11 +9134,11 @@
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>3.5650909090909088E-3</v>
+        <v>2.5168831168831168E-4</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
-        <v>0.72975017635830897</v>
+        <v>-2.1214358815296808E-2</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -8954,7 +9148,7 @@
       </c>
       <c r="M61">
         <f t="shared" si="2"/>
-        <v>13490.188953488372</v>
+        <v>191084.5588235294</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
@@ -8963,11 +9157,11 @@
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>3.6276363636363637E-3</v>
+        <v>2.5610389610389615E-4</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
-        <v>0.99945126756040126</v>
+        <v>-7.6628628573469304E-2</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -8977,7 +9171,7 @@
       </c>
       <c r="M62">
         <f t="shared" si="2"/>
-        <v>13740.007267441861</v>
+        <v>194623.16176470587</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
@@ -8986,11 +9180,11 @@
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>3.6901818181818181E-3</v>
+        <v>2.6051948051948056E-4</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
-        <v>0.68287977698735558</v>
+        <v>-0.13180702668836025</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -9000,7 +9194,7 @@
       </c>
       <c r="M63">
         <f t="shared" si="2"/>
-        <v>13989.825581395349</v>
+        <v>198161.76470588235</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
@@ -9009,11 +9203,11 @@
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>3.7527272727272726E-3</v>
+        <v>2.6493506493506497E-4</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
-        <v>-3.4265211154653925E-2</v>
+        <v>-0.18657970776825072</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -9023,7 +9217,7 @@
       </c>
       <c r="M64">
         <f t="shared" si="2"/>
-        <v>14239.643895348838</v>
+        <v>201700.3676470588</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
@@ -9032,11 +9226,11 @@
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>3.815272727272727E-3</v>
+        <v>2.6935064935064938E-4</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
-        <v>-0.73131041608488201</v>
+        <v>-0.24077807526464745</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -9046,7 +9240,7 @@
       </c>
       <c r="M65">
         <f t="shared" si="2"/>
-        <v>14489.462209302326</v>
+        <v>205238.97058823527</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
@@ -9055,11 +9249,11 @@
       </c>
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>3.8778181818181819E-3</v>
+        <v>2.737662337662338E-4</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
-        <v>-0.99937297860605745</v>
+        <v>-0.2942353004316568</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -9069,7 +9263,7 @@
       </c>
       <c r="M66">
         <f t="shared" si="2"/>
-        <v>14739.280523255813</v>
+        <v>208777.57352941175</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
@@ -9078,11 +9272,11 @@
       </c>
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>3.9403636363636359E-3</v>
+        <v>2.7818181818181821E-4</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
-        <v>-0.68120888321940343</v>
+        <v>-0.34678683584385617</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -9092,7 +9286,7 @@
       </c>
       <c r="M67">
         <f t="shared" si="2"/>
-        <v>14989.098837209302</v>
+        <v>212316.17647058822</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
@@ -9101,11 +9295,11 @@
       </c>
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>4.0029090909090908E-3</v>
+        <v>2.8259740259740262E-4</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
-        <v>3.6548572700025428E-2</v>
+        <v>-0.39827092189200591</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -9115,7 +9309,7 @@
       </c>
       <c r="M68">
         <f t="shared" si="2"/>
-        <v>15238.91715116279</v>
+        <v>215854.7794117647</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
@@ -9124,11 +9318,11 @@
       </c>
       <c r="B69">
         <f t="shared" ref="B69:B131" si="3">A69*$B$1</f>
-        <v>4.0654545454545457E-3</v>
+        <v>2.8701298701298703E-4</v>
       </c>
       <c r="C69">
         <f t="shared" ref="C69:C131" si="4">SIN(2*PI()*$B$2*B69)</f>
-        <v>0.7328668381631317</v>
+        <v>-0.44852908469754255</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -9138,7 +9332,7 @@
       </c>
       <c r="M69">
         <f t="shared" si="2"/>
-        <v>15488.735465116279</v>
+        <v>219393.38235294115</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
@@ -9147,11 +9341,11 @@
       </c>
       <c r="B70">
         <f t="shared" si="3"/>
-        <v>4.1279999999999997E-3</v>
+        <v>2.9142857142857144E-4</v>
       </c>
       <c r="C70">
         <f t="shared" si="4"/>
-        <v>0.99928947264058965</v>
+        <v>-0.49740662391322182</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -9161,7 +9355,7 @@
       </c>
       <c r="M70">
         <f t="shared" si="2"/>
-        <v>15738.553779069767</v>
+        <v>222931.98529411762</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
@@ -9170,11 +9364,11 @@
       </c>
       <c r="B71">
         <f t="shared" si="3"/>
-        <v>4.1905454545454546E-3</v>
+        <v>2.9584415584415585E-4</v>
       </c>
       <c r="C71">
         <f t="shared" si="4"/>
-        <v>0.67953443334737085</v>
+        <v>-0.54475308890839824</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -9186,11 +9380,11 @@
       </c>
       <c r="B72">
         <f t="shared" si="3"/>
-        <v>4.2530909090909086E-3</v>
+        <v>3.0025974025974027E-4</v>
       </c>
       <c r="C72">
         <f t="shared" si="4"/>
-        <v>-3.8831743451440491E-2</v>
+        <v>-0.59042274187319743</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -9202,11 +9396,11 @@
       </c>
       <c r="B73">
         <f t="shared" si="3"/>
-        <v>4.3156363636363635E-3</v>
+        <v>3.0467532467532468E-4</v>
       </c>
       <c r="C73">
         <f t="shared" si="4"/>
-        <v>-0.73441943446808267</v>
+        <v>-0.63427500641608803</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -9218,11 +9412,11 @@
       </c>
       <c r="B74">
         <f t="shared" si="3"/>
-        <v>4.3781818181818184E-3</v>
+        <v>3.0909090909090909E-4</v>
       </c>
       <c r="C74">
         <f t="shared" si="4"/>
-        <v>-0.99920075009992171</v>
+        <v>-0.67617490027401916</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -9234,11 +9428,11 @@
       </c>
       <c r="B75">
         <f t="shared" si="3"/>
-        <v>4.4407272727272724E-3</v>
+        <v>3.1350649350649355E-4</v>
       </c>
       <c r="C75">
         <f t="shared" si="4"/>
-        <v>-0.67785643611237278</v>
+        <v>-0.71599345080319499</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -9250,11 +9444,11 @@
       </c>
       <c r="B76">
         <f t="shared" si="3"/>
-        <v>4.5032727272727273E-3</v>
+        <v>3.1792207792207797E-4</v>
       </c>
       <c r="C76">
         <f t="shared" si="4"/>
-        <v>4.1114711490134064E-2</v>
+        <v>-0.75360809197155576</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -9266,11 +9460,11 @@
       </c>
       <c r="B77">
         <f t="shared" si="3"/>
-        <v>4.5658181818181813E-3</v>
+        <v>3.2233766233766238E-4</v>
       </c>
       <c r="C77">
         <f t="shared" si="4"/>
-        <v>0.73596819689475501</v>
+        <v>-0.78890304163098079</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -9282,11 +9476,11 @@
       </c>
       <c r="B78">
         <f t="shared" si="3"/>
-        <v>4.6283636363636362E-3</v>
+        <v>3.2675324675324679E-4</v>
       </c>
       <c r="C78">
         <f t="shared" si="4"/>
-        <v>0.99910681144721147</v>
+        <v>-0.82176965790792089</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -9298,11 +9492,11 @@
       </c>
       <c r="B79">
         <f t="shared" si="3"/>
-        <v>4.6909090909090911E-3</v>
+        <v>3.311688311688312E-4</v>
       </c>
       <c r="C79">
         <f t="shared" si="4"/>
-        <v>0.67617490027402161</v>
+        <v>-0.85210677361545673</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -9314,11 +9508,11 @@
       </c>
       <c r="B80">
         <f t="shared" si="3"/>
-        <v>4.7534545454545451E-3</v>
+        <v>3.3558441558441561E-4</v>
       </c>
       <c r="C80">
         <f t="shared" si="4"/>
-        <v>-4.3397464898321206E-2</v>
+        <v>-0.87982100765741533</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -9330,11 +9524,11 @@
       </c>
       <c r="B81">
         <f t="shared" si="3"/>
-        <v>4.816E-3</v>
+        <v>3.4000000000000002E-4</v>
       </c>
       <c r="C81">
         <f t="shared" si="4"/>
-        <v>-0.73751311735816871</v>
+        <v>-0.90482705246601935</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -9346,11 +9540,11 @@
       </c>
       <c r="B82">
         <f t="shared" si="3"/>
-        <v>4.8785454545454549E-3</v>
+        <v>3.4441558441558444E-4</v>
       </c>
       <c r="C82">
         <f t="shared" si="4"/>
-        <v>-0.99900765717284468</v>
+        <v>-0.92704793658829177</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -9362,11 +9556,11 @@
       </c>
       <c r="B83">
         <f t="shared" si="3"/>
-        <v>4.9410909090909089E-3</v>
+        <v>3.4883116883116885E-4</v>
       </c>
       <c r="C83">
         <f t="shared" si="4"/>
-        <v>-0.67448983461042811</v>
+        <v>-0.94641526161295064</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -9378,11 +9572,11 @@
       </c>
       <c r="B84">
         <f t="shared" si="3"/>
-        <v>5.0036363636363637E-3</v>
+        <v>3.5324675324675326E-4</v>
       </c>
       <c r="C84">
         <f t="shared" si="4"/>
-        <v>4.5679991759415513E-2</v>
+        <v>-0.9628694127085089</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -9394,11 +9588,11 @@
       </c>
       <c r="B85">
         <f t="shared" si="3"/>
-        <v>5.0661818181818178E-3</v>
+        <v>3.5766233766233767E-4</v>
       </c>
       <c r="C85">
         <f t="shared" si="4"/>
-        <v>0.73905418779338972</v>
+        <v>-0.9763597421245116</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -9410,11 +9604,11 @@
       </c>
       <c r="B86">
         <f t="shared" si="3"/>
-        <v>5.1287272727272726E-3</v>
+        <v>3.6207792207792208E-4</v>
       </c>
       <c r="C86">
         <f t="shared" si="4"/>
-        <v>0.99890328779443582</v>
+        <v>-0.98684472509107801</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -9426,11 +9620,11 @@
       </c>
       <c r="B87">
         <f t="shared" si="3"/>
-        <v>5.1912727272727275E-3</v>
+        <v>3.6649350649350649E-4</v>
       </c>
       <c r="C87">
         <f t="shared" si="4"/>
-        <v>0.67280124791808804</v>
+        <v>-0.99429208763687249</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -9442,11 +9636,11 @@
       </c>
       <c r="B88">
         <f t="shared" si="3"/>
-        <v>5.2538181818181815E-3</v>
+        <v>3.7090909090909096E-4</v>
       </c>
       <c r="C88">
         <f t="shared" si="4"/>
-        <v>-4.7962280157963534E-2</v>
+        <v>-0.99867890593206143</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -9458,11 +9652,11 @@
       </c>
       <c r="B89">
         <f t="shared" si="3"/>
-        <v>5.3163636363636364E-3</v>
+        <v>3.7532467532467537E-4</v>
       </c>
       <c r="C89">
         <f t="shared" si="4"/>
-        <v>-0.74059140015560199</v>
+        <v>-0.99999167685047219</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -9474,11 +9668,11 @@
       </c>
       <c r="B90">
         <f t="shared" si="3"/>
-        <v>5.3789090909090904E-3</v>
+        <v>3.7974025974025978E-4</v>
       </c>
       <c r="C90">
         <f t="shared" si="4"/>
-        <v>-0.99879370385682154</v>
+        <v>-0.99822635953375283</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -9490,11 +9684,11 @@
       </c>
       <c r="B91">
         <f t="shared" si="3"/>
-        <v>5.4414545454545453E-3</v>
+        <v>3.841558441558442E-4</v>
       </c>
       <c r="C91">
         <f t="shared" si="4"/>
-        <v>-0.67110914901193552</v>
+        <v>-0.99338838782959382</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -9506,11 +9700,11 @@
       </c>
       <c r="B92">
         <f t="shared" si="3"/>
-        <v>5.5040000000000002E-3</v>
+        <v>3.8857142857142861E-4</v>
       </c>
       <c r="C92">
         <f t="shared" si="4"/>
-        <v>5.024431817977084E-2</v>
+        <v>-0.98549265356572668</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -9522,11 +9716,11 @@
       </c>
       <c r="B93">
         <f t="shared" si="3"/>
-        <v>5.5665454545454542E-3</v>
+        <v>3.9298701298701302E-4</v>
       </c>
       <c r="C93">
         <f t="shared" si="4"/>
-        <v>0.74212474642010551</v>
+        <v>-0.97456346071118227</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -9538,11 +9732,11 @@
       </c>
       <c r="B94">
         <f t="shared" si="3"/>
-        <v>5.6290909090909091E-3</v>
+        <v>3.9740259740259743E-4</v>
       </c>
       <c r="C94">
         <f t="shared" si="4"/>
-        <v>0.99867890593206166</v>
+        <v>-0.96063445056590702</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -9554,11 +9748,11 @@
       </c>
       <c r="B95">
         <f t="shared" si="3"/>
-        <v>5.6916363636363631E-3</v>
+        <v>4.0181818181818184E-4</v>
       </c>
       <c r="C95">
         <f t="shared" si="4"/>
-        <v>0.66941354672519249</v>
+        <v>-0.94374849820901208</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -9570,11 +9764,11 @@
       </c>
       <c r="B96">
         <f t="shared" si="3"/>
-        <v>5.754181818181818E-3</v>
+        <v>4.0623376623376625E-4</v>
       </c>
       <c r="C96">
         <f t="shared" si="4"/>
-        <v>-5.2526093911935856E-2</v>
+        <v>-0.92395758052439747</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -9586,11 +9780,11 @@
       </c>
       <c r="B97">
         <f t="shared" si="3"/>
-        <v>5.8167272727272729E-3</v>
+        <v>4.1064935064935067E-4</v>
       </c>
       <c r="C97">
         <f t="shared" si="4"/>
-        <v>-0.74365421858241576</v>
+        <v>-0.90132261620998577</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -9602,11 +9796,11 @@
       </c>
       <c r="B98">
         <f t="shared" si="3"/>
-        <v>5.8792727272727269E-3</v>
+        <v>4.1506493506493508E-4</v>
       </c>
       <c r="C98">
         <f t="shared" si="4"/>
-        <v>-0.9985588946194347</v>
+        <v>-0.875913278263035</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -9618,11 +9812,11 @@
       </c>
       <c r="B99">
         <f t="shared" si="3"/>
-        <v>5.9418181818181818E-3</v>
+        <v>4.1948051948051949E-4</v>
       </c>
       <c r="C99">
         <f t="shared" si="4"/>
-        <v>-0.66771444990936357</v>
+        <v>-0.84780777951871922</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -9634,11 +9828,11 @@
       </c>
       <c r="B100">
         <f t="shared" si="3"/>
-        <v>6.0043636363636358E-3</v>
+        <v>4.2389610389610395E-4</v>
       </c>
       <c r="C100">
         <f t="shared" si="4"/>
-        <v>5.4807595442954632E-2</v>
+        <v>-0.81709263190211612</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -9650,11 +9844,11 @@
       </c>
       <c r="B101">
         <f t="shared" si="3"/>
-        <v>6.0669090909090907E-3</v>
+        <v>4.2831168831168837E-4</v>
       </c>
       <c r="C101">
         <f t="shared" si="4"/>
-        <v>0.74517980865824363</v>
+        <v>-0.7838623801346567</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -9666,11 +9860,11 @@
       </c>
       <c r="B102">
         <f t="shared" si="3"/>
-        <v>6.1294545454545456E-3</v>
+        <v>4.3272727272727278E-4</v>
       </c>
       <c r="C102">
         <f t="shared" si="4"/>
-        <v>0.99843367054543253</v>
+        <v>-0.7482193107147016</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -9682,11 +9876,11 @@
       </c>
       <c r="B103">
         <f t="shared" si="3"/>
-        <v>6.1919999999999996E-3</v>
+        <v>4.3714285714285719E-4</v>
       </c>
       <c r="C103">
         <f t="shared" si="4"/>
-        <v>0.66601186743425977</v>
+        <v>-0.71027313706805684</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -9698,11 +9892,11 @@
       </c>
       <c r="B104">
         <f t="shared" si="3"/>
-        <v>6.2545454545454545E-3</v>
+        <v>4.415584415584416E-4</v>
       </c>
       <c r="C104">
         <f t="shared" si="4"/>
-        <v>-5.7088810862754608E-2</v>
+        <v>-0.6701406618375596</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -9714,11 +9908,11 @@
       </c>
       <c r="B105">
         <f t="shared" si="3"/>
-        <v>6.3170909090909094E-3</v>
+        <v>4.4597402597402601E-4</v>
       </c>
       <c r="C105">
         <f t="shared" si="4"/>
-        <v>-0.7467015086835751</v>
+        <v>-0.62794541735124088</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -9730,11 +9924,11 @@
       </c>
       <c r="B106">
         <f t="shared" si="3"/>
-        <v>6.3796363636363634E-3</v>
+        <v>4.5038961038961042E-4</v>
       </c>
       <c r="C106">
         <f t="shared" si="4"/>
-        <v>-0.99830323436376189</v>
+        <v>-0.58381728537575706</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -9746,11 +9940,11 @@
       </c>
       <c r="B107">
         <f t="shared" si="3"/>
-        <v>6.4421818181818183E-3</v>
+        <v>4.5480519480519484E-4</v>
       </c>
       <c r="C107">
         <f t="shared" si="4"/>
-        <v>-0.66430580818781404</v>
+        <v>-0.53789209732552679</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -9762,11 +9956,11 @@
       </c>
       <c r="B108">
         <f t="shared" si="3"/>
-        <v>6.5047272727272723E-3</v>
+        <v>4.5922077922077925E-4</v>
       </c>
       <c r="C108">
         <f t="shared" si="4"/>
-        <v>5.9369728262728419E-2</v>
+        <v>-0.49031121615816797</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -9778,11 +9972,11 @@
       </c>
       <c r="B109">
         <f t="shared" si="3"/>
-        <v>6.5672727272727272E-3</v>
+        <v>4.6363636363636366E-4</v>
       </c>
       <c r="C109">
         <f t="shared" si="4"/>
-        <v>0.74821931071469394</v>
+        <v>-0.44122110124322145</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -9794,11 +9988,11 @@
       </c>
       <c r="B110">
         <f t="shared" si="3"/>
-        <v>6.629818181818182E-3</v>
+        <v>4.6805194805194807E-4</v>
       </c>
       <c r="C110">
         <f t="shared" si="4"/>
-        <v>0.99816758675533435</v>
+        <v>-0.39077285754353874</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -9810,11 +10004,11 @@
       </c>
       <c r="B111">
         <f t="shared" si="3"/>
-        <v>6.692363636363636E-3</v>
+        <v>4.7246753246753248E-4</v>
       </c>
       <c r="C111">
         <f t="shared" si="4"/>
-        <v>0.66259628107616175</v>
+        <v>-0.33912177049699727</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -9826,11 +10020,11 @@
       </c>
       <c r="B112">
         <f t="shared" si="3"/>
-        <v>6.7549090909090909E-3</v>
+        <v>4.7688311688311689E-4</v>
       </c>
       <c r="C112">
         <f t="shared" si="4"/>
-        <v>-6.1650335735838648E-2</v>
+        <v>-0.2864268280302486</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -9842,11 +10036,11 @@
       </c>
       <c r="B113">
         <f t="shared" si="3"/>
-        <v>6.8174545454545449E-3</v>
+        <v>4.8129870129870136E-4</v>
       </c>
       <c r="C113">
         <f t="shared" si="4"/>
-        <v>-0.7497332068282514</v>
+        <v>-0.23285023117577217</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -9858,11 +10052,11 @@
       </c>
       <c r="B114">
         <f t="shared" si="3"/>
-        <v>6.8799999999999998E-3</v>
+        <v>4.8571428571428577E-4</v>
       </c>
       <c r="C114">
         <f t="shared" si="4"/>
-        <v>-0.99802672842827211</v>
+        <v>-0.17855689479863687</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -9874,11 +10068,11 @@
       </c>
       <c r="B115">
         <f t="shared" si="3"/>
-        <v>6.9425454545454547E-3</v>
+        <v>4.9012987012987013E-4</v>
       </c>
       <c r="C115">
         <f t="shared" si="4"/>
-        <v>-0.66088329502349952</v>
+        <v>-0.123713939969764</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -9890,11 +10084,11 @@
       </c>
       <c r="B116">
         <f t="shared" si="3"/>
-        <v>7.0050909090909087E-3</v>
+        <v>4.9454545454545454E-4</v>
       </c>
       <c r="C116">
         <f t="shared" si="4"/>
-        <v>6.393062137665162E-2</v>
+        <v>-6.849017954824671E-2</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -9906,11 +10100,11 @@
       </c>
       <c r="B117">
         <f t="shared" si="3"/>
-        <v>7.0676363636363636E-3</v>
+        <v>4.9896103896103895E-4</v>
       </c>
       <c r="C117">
         <f t="shared" si="4"/>
-        <v>0.75124318912128873</v>
+        <v>-1.3055598556147987E-2</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -9922,11 +10116,11 @@
       </c>
       <c r="B118">
         <f t="shared" si="3"/>
-        <v>7.1301818181818176E-3</v>
+        <v>5.0337662337662336E-4</v>
       </c>
       <c r="C118">
         <f t="shared" si="4"/>
-        <v>0.99788066011789434</v>
+        <v>4.2419169054747352E-2</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -9938,11 +10132,11 @@
       </c>
       <c r="B119">
         <f t="shared" si="3"/>
-        <v>7.1927272727272725E-3</v>
+        <v>5.0779220779220778E-4</v>
       </c>
       <c r="C119">
         <f t="shared" si="4"/>
-        <v>0.65916685897211214</v>
+        <v>9.7763365633669053E-2</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -9954,11 +10148,11 @@
       </c>
       <c r="B120">
         <f t="shared" si="3"/>
-        <v>7.2552727272727274E-3</v>
+        <v>5.122077922077923E-4</v>
       </c>
       <c r="C120">
         <f t="shared" si="4"/>
-        <v>-6.6210573281456214E-2</v>
+        <v>0.15280663544235026</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -9970,11 +10164,11 @@
       </c>
       <c r="B121">
         <f t="shared" si="3"/>
-        <v>7.3178181818181814E-3</v>
+        <v>5.1662337662337671E-4</v>
       </c>
       <c r="C121">
         <f t="shared" si="4"/>
-        <v>-0.75274924971125945</v>
+        <v>0.20737954902938052</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -9986,11 +10180,11 @@
       </c>
       <c r="B122">
         <f t="shared" si="3"/>
-        <v>7.3803636363636363E-3</v>
+        <v>5.2103896103896112E-4</v>
       </c>
       <c r="C122">
         <f t="shared" si="4"/>
-        <v>-0.99772938258671795</v>
+        <v>0.26131412475335447</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -10002,11 +10196,11 @@
       </c>
       <c r="B123">
         <f t="shared" si="3"/>
-        <v>7.4429090909090912E-3</v>
+        <v>5.2545454545454553E-4</v>
       </c>
       <c r="C123">
         <f t="shared" si="4"/>
-        <v>-0.65744698188228401</v>
+        <v>0.31444434584948794</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -10018,11 +10212,11 @@
       </c>
       <c r="B124">
         <f t="shared" si="3"/>
-        <v>7.5054545454545452E-3</v>
+        <v>5.2987012987012994E-4</v>
       </c>
       <c r="C124">
         <f t="shared" si="4"/>
-        <v>6.8490179548226851E-2</v>
+        <v>0.36660667144812081</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -10034,11 +10228,11 @@
       </c>
       <c r="B125">
         <f t="shared" si="3"/>
-        <v>7.5680000000000001E-3</v>
+        <v>5.3428571428571436E-4</v>
       </c>
       <c r="C125">
         <f t="shared" si="4"/>
-        <v>0.7542513807360991</v>
+        <v>0.41764053997213119</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -10050,11 +10244,11 @@
       </c>
       <c r="B126">
         <f t="shared" si="3"/>
-        <v>7.6305454545454541E-3</v>
+        <v>5.3870129870129877E-4</v>
       </c>
       <c r="C126">
         <f t="shared" si="4"/>
-        <v>0.99757289662445581</v>
+        <v>0.46738886336375562</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -10066,11 +10260,11 @@
       </c>
       <c r="B127">
         <f t="shared" si="3"/>
-        <v>7.693090909090909E-3</v>
+        <v>5.4311688311688318E-4</v>
       </c>
       <c r="C127">
         <f t="shared" si="4"/>
-        <v>0.65572367273227306</v>
+        <v>0.51569851061951333</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -10082,11 +10276,11 @@
       </c>
       <c r="B128">
         <f t="shared" si="3"/>
-        <v>7.7556363636363639E-3</v>
+        <v>5.4753246753246759E-4</v>
       </c>
       <c r="C128">
         <f t="shared" si="4"/>
-        <v>-7.0769428276813109E-2</v>
+        <v>0.56242077914486777</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -10098,11 +10292,11 @@
       </c>
       <c r="B129">
         <f t="shared" si="3"/>
-        <v>7.8181818181818179E-3</v>
+        <v>5.51948051948052E-4</v>
       </c>
       <c r="C129">
         <f t="shared" si="4"/>
-        <v>-0.75574957435424728</v>
+        <v>0.60741185247774776</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -10114,11 +10308,11 @@
       </c>
       <c r="B130">
         <f t="shared" si="3"/>
-        <v>7.8807272727272719E-3</v>
+        <v>5.5636363636363641E-4</v>
       </c>
       <c r="C130">
         <f t="shared" si="4"/>
-        <v>-0.9974112030480099</v>
+        <v>0.650533242971987</v>
       </c>
       <c r="D130">
         <v>0</v>
@@ -10130,11 +10324,11 @@
       </c>
       <c r="B131">
         <f t="shared" si="3"/>
-        <v>7.9432727272727276E-3</v>
+        <v>5.6077922077922083E-4</v>
       </c>
       <c r="C131">
         <f t="shared" si="4"/>
-        <v>-0.65399694051822188</v>
+        <v>0.69165221807807031</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -10147,12 +10341,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28DF378C-AF84-49EE-8EF2-209CED79A22D}">
   <dimension ref="A2:E513"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>